<commit_message>
Fixed tests and test data for the Study.code removal.
Files checked in: DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table_newsample.xlsx DataRepo/data/tests/small_obob/small_obob_study.xlsx DataRepo/data/tests/study_doc_versions/study_v3.xlsx DataRepo/data/tests/submission_v3/multitracer_v3/study.xlsx DataRepo/data/tests/submission_v3/multitracer_v3/study_missing_data.xlsx DataRepo/data/tests/submission_v3/study_no_defs.xlsx DataRepo/data/tests/submission_v3/study_with_autofill_seeds.xlsx DataRepo/loaders/study_loader.py DataRepo/tests/management/commands/test_load_studies.py DataRepo/tests/views/upload/test_validation.py
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/small_obob/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78474804-941F-6B45-92A5-24FF911A5915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A46F09BC-FC88-9148-BB58-64E5D2AE771A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="1520" windowWidth="29900" windowHeight="20220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,80 +46,7 @@
     <author>TraceBase Dev Team</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{C8F73FAE-0063-184D-AE84-904817F8C9D8}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Courier"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">A 2 to 6 character unique readable alphanumeric code for the study, to be used
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Courier"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">as a prefix for animal names, sample names, etc if necessary, to make them
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Courier"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">unique.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Courier"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Courier"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Must be unique.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Courier"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Courier"/>
-            <family val="2"/>
-          </rPr>
-          <t>Optional.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{9DD3C0F6-643F-C646-9957-604AAD2D5A2E}">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9DD3C0F6-643F-C646-9957-604AAD2D5A2E}">
       <text>
         <r>
           <rPr>
@@ -135,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{13ED60A2-33CC-984B-A004-5ADFF55D03F9}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{13ED60A2-33CC-984B-A004-5ADFF55D03F9}">
       <text>
         <r>
           <rPr>
@@ -1206,7 +1133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="139">
   <si>
     <t>Infusate</t>
   </si>
@@ -1662,16 +1589,10 @@
     <t>1972-11-24</t>
   </si>
   <si>
-    <t>Study ID</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>A description</t>
-  </si>
-  <si>
-    <t>obob</t>
   </si>
 </sst>
 </file>
@@ -2316,51 +2237,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C61425D-F23C-6F4F-8608-324522C2138E}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14">
+    <row r="1" spans="1:2" ht="14">
       <c r="A1" s="22" t="s">
         <v>137</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>138</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="20" t="s">
-        <v>140</v>
-      </c>
-      <c r="B2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1">
-    <cfRule type="notContainsErrors" dxfId="7" priority="1">
+    <cfRule type="notContainsErrors" dxfId="6" priority="2">
       <formula>NOT(ISERROR(A1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="notContainsErrors" dxfId="6" priority="2">
+    <cfRule type="notContainsErrors" dxfId="5" priority="3">
       <formula>NOT(ISERROR(B1))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1">
-    <cfRule type="notContainsErrors" dxfId="5" priority="3">
-      <formula>NOT(ISERROR(C1))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Transferred legacy test "test_accucor_load_sample_prefix" to v3 code.
Files checked in: DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table_newsample.xlsx DataRepo/management/commands/load_study.py DataRepo/tests/management/commands/legacy/test_load_accucor_msruns.py DataRepo/tests/management/commands/test_load_peak_annotations.py
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/small_obob/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30FB41AE-F000-CF4C-861D-2854CB51EF87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F619E11B-1022-5146-B04E-67CE3C3A4729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1685,7 +1685,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="351">
   <si>
     <t>Infusate</t>
   </si>
@@ -2778,6 +2778,9 @@
   </si>
   <si>
     <t>3-Phosphoglycerate; Glycerate 3-phosphate; 3-PG</t>
+  </si>
+  <si>
+    <t>newsample</t>
   </si>
 </sst>
 </file>
@@ -27699,9 +27702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD2DCCD-0178-094D-9522-9414A02DC911}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
@@ -27947,8 +27948,8 @@
       <c r="A17" t="s">
         <v>104</v>
       </c>
-      <c r="B17" t="s">
-        <v>104</v>
+      <c r="B17" s="20" t="s">
+        <v>350</v>
       </c>
       <c r="D17" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
Transferred legacy test "test_accucor_load_sample_prefix_missing" to v3.
Files checked in: DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table_newsample.xlsx DataRepo/tests/management/commands/legacy/test_load_accucor_msruns.py DataRepo/tests/management/commands/test_load_peak_annotations.py DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table_newsample_missing_prefix.xlsx
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/small_obob/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F619E11B-1022-5146-B04E-67CE3C3A4729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E62946-2DF9-634F-BC35-227409DEF643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
     <sheet name="Compounds" sheetId="12" r:id="rId11"/>
     <sheet name="Infusions" sheetId="5" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27702,7 +27702,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD2DCCD-0178-094D-9522-9414A02DC911}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>

</xml_diff>

<commit_message>
Fixed a mistaken edit.
Files checked in: DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/small_obob/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E62946-2DF9-634F-BC35-227409DEF643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B170C642-B36E-654D-8BD2-206F3F5F44E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1685,7 +1685,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="350">
   <si>
     <t>Infusate</t>
   </si>
@@ -2778,9 +2778,6 @@
   </si>
   <si>
     <t>3-Phosphoglycerate; Glycerate 3-phosphate; 3-PG</t>
-  </si>
-  <si>
-    <t>newsample</t>
   </si>
 </sst>
 </file>
@@ -27703,7 +27700,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -27951,7 +27948,7 @@
         <v>104</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>350</v>
+        <v>104</v>
       </c>
       <c r="D17" t="s">
         <v>125</v>
@@ -27972,7 +27969,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Each sample name must be unique" sqref="A2:B17" xr:uid="{F169F778-8480-4947-ABEB-D876FA8E756B}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Each sample name must be unique" sqref="A2:A17 B2:B16" xr:uid="{F169F778-8480-4947-ABEB-D876FA8E756B}">
       <formula1>COUNTIF($A:$A,"="&amp;A2)  &lt; 2</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Transferred legacy test "test_accucor_load_in_debug" to v3 code.
Files checked in: DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx DataRepo/tests/management/commands/legacy/test_load_accucor_msruns.py DataRepo/tests/management/commands/test_load_peak_annotations.py
</commit_message>
<xml_diff>
--- a/DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
+++ b/DataRepo/data/tests/small_obob/small_obob_animal_and_sample_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rleach/PROJECT-local/TRACEBASE/tracebase/DataRepo/data/tests/small_obob/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B170C642-B36E-654D-8BD2-206F3F5F44E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF05B11-91C3-0A4C-A366-4230B483E951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1685,7 +1685,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="353">
   <si>
     <t>Infusate</t>
   </si>
@@ -2778,6 +2778,15 @@
   </si>
   <si>
     <t>3-Phosphoglycerate; Glycerate 3-phosphate; 3-PG</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t>skip</t>
+  </si>
+  <si>
+    <t>small_obob_maven_6eaas_inf_blank_sample.xlsx</t>
   </si>
 </sst>
 </file>
@@ -27697,10 +27706,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCD2DCCD-0178-094D-9522-9414A02DC911}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -27708,7 +27717,7 @@
     <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5" customWidth="1"/>
     <col min="5" max="5" width="46.5" customWidth="1"/>
     <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
   </cols>
@@ -27943,7 +27952,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>104</v>
       </c>
@@ -27955,6 +27964,23 @@
       </c>
       <c r="E17" s="20" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>352</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -27969,7 +27995,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Each sample name must be unique" sqref="A2:A17 B2:B16" xr:uid="{F169F778-8480-4947-ABEB-D876FA8E756B}">
+    <dataValidation type="custom" allowBlank="1" showDropDown="1" showInputMessage="1" prompt="Each sample name must be unique" sqref="A2:A18 B2:B16" xr:uid="{F169F778-8480-4947-ABEB-D876FA8E756B}">
       <formula1>COUNTIF($A:$A,"="&amp;A2)  &lt; 2</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>